<commit_message>
tambah 9v ke vin sama re kalibrasi lagi
</commit_message>
<xml_diff>
--- a/Arduino-Bluetooth/docs 2nd Approach/ANOVA_chauvenet.xlsx
+++ b/Arduino-Bluetooth/docs 2nd Approach/ANOVA_chauvenet.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,50 +434,60 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>sum_sq</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>df</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>PR(&gt;F)</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>977.528706763984</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>voltage</t>
+        </is>
       </c>
       <c r="B2" t="n">
+        <v>0.5192140393846513</v>
+      </c>
+      <c r="C2" t="n">
         <v>8</v>
       </c>
-      <c r="C2" t="n">
-        <v>152.036683201402</v>
-      </c>
       <c r="D2" t="n">
-        <v>1.690552261972696e-239</v>
+        <v>6.92128216846749</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4.052735474009534e-09</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>6548.505050720132</v>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Residual</t>
+        </is>
       </c>
       <c r="B3" t="n">
-        <v>8148</v>
-      </c>
-      <c r="C3" t="inlineStr"/>
+        <v>71.24742524617514</v>
+      </c>
+      <c r="C3" t="n">
+        <v>7598</v>
+      </c>
       <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
ading new chauvenet + std
</commit_message>
<xml_diff>
--- a/Arduino-Bluetooth/docs 2nd Approach/ANOVA_chauvenet.xlsx
+++ b/Arduino-Bluetooth/docs 2nd Approach/ANOVA_chauvenet.xlsx
@@ -462,16 +462,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5192140393846513</v>
+        <v>157.6633739787549</v>
       </c>
       <c r="C2" t="n">
         <v>8</v>
       </c>
       <c r="D2" t="n">
-        <v>6.92128216846749</v>
+        <v>782.0969401757909</v>
       </c>
       <c r="E2" t="n">
-        <v>4.052735474009534e-09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -481,10 +481,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>71.24742524617514</v>
+        <v>203.0269105549284</v>
       </c>
       <c r="C3" t="n">
-        <v>7598</v>
+        <v>8057</v>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>

</xml_diff>